<commit_message>
Second Template Fix – Scroll to Top
</commit_message>
<xml_diff>
--- a/CDAP Template.xlsx
+++ b/CDAP Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshaho/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CE2566-6225-A346-9883-DE23C53F18E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A41E12-39E6-6B40-90A3-3E26E9C4F80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="1480" windowWidth="25600" windowHeight="15540" xr2:uid="{2B29D527-18C8-44C8-9ECB-45F01A2C0AD6}"/>
   </bookViews>
@@ -716,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -862,7 +862,6 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2313,9 +2312,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C1937D-FCA4-432E-A3D1-AC32563B1CCF}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F30" sqref="F30:F34"/>
     </sheetView>
   </sheetViews>
@@ -2588,7 +2587,7 @@
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2604,7 +2603,7 @@
       </c>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2620,7 +2619,7 @@
       </c>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2636,7 +2635,7 @@
       </c>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="45.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2652,7 +2651,7 @@
       </c>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2668,7 +2667,7 @@
       </c>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -2684,7 +2683,7 @@
       </c>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2700,7 +2699,7 @@
       </c>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2716,7 +2715,7 @@
       </c>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -2732,7 +2731,7 @@
       </c>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -2748,7 +2747,7 @@
       </c>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -2764,7 +2763,7 @@
       </c>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -2779,9 +2778,8 @@
         <v>3.23</v>
       </c>
       <c r="F28" s="9"/>
-      <c r="G28" s="53"/>
-    </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -2796,9 +2794,8 @@
         <v>3.3</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="53"/>
-    </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -2813,9 +2810,8 @@
         <v>3.51</v>
       </c>
       <c r="F30" s="9"/>
-      <c r="G30" s="53"/>
-    </row>
-    <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -2830,9 +2826,8 @@
         <v>3.51</v>
       </c>
       <c r="F31" s="9"/>
-      <c r="G31" s="53"/>
-    </row>
-    <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -2847,9 +2842,8 @@
         <v>3.53</v>
       </c>
       <c r="F32" s="9"/>
-      <c r="G32" s="53"/>
-    </row>
-    <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -2864,9 +2858,8 @@
         <v>3.48</v>
       </c>
       <c r="F33" s="9"/>
-      <c r="G33" s="53"/>
-    </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -2881,9 +2874,8 @@
         <v>3.36</v>
       </c>
       <c r="F34" s="9"/>
-      <c r="G34" s="53"/>
-    </row>
-    <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -2898,9 +2890,8 @@
         <v>3.28</v>
       </c>
       <c r="F35" s="9"/>
-      <c r="G35" s="53"/>
-    </row>
-    <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -2915,9 +2906,8 @@
         <v>3.51</v>
       </c>
       <c r="F36" s="9"/>
-      <c r="G36" s="53"/>
-    </row>
-    <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -2933,7 +2923,7 @@
       </c>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -2949,7 +2939,7 @@
       </c>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -2965,7 +2955,7 @@
       </c>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -2981,7 +2971,7 @@
       </c>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -2997,7 +2987,7 @@
       </c>
       <c r="F41" s="9"/>
     </row>
-    <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -3360,7 +3350,7 @@
     <col min="16" max="16384" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="33" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3407,7 +3397,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -3454,7 +3444,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -3501,7 +3491,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -3548,7 +3538,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A5" s="26">
         <v>4</v>
       </c>
@@ -3595,7 +3585,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="26">
         <v>5</v>
       </c>
@@ -3642,7 +3632,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A7" s="26">
         <v>6</v>
       </c>
@@ -3689,7 +3679,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="26">
         <v>7</v>
       </c>
@@ -3736,7 +3726,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="33" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A9" s="26">
         <v>8</v>
       </c>
@@ -3783,7 +3773,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A10" s="26">
         <v>9</v>
       </c>
@@ -3830,7 +3820,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="33" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A11" s="26">
         <v>10</v>
       </c>
@@ -3877,7 +3867,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A12" s="26">
         <v>11</v>
       </c>
@@ -3924,7 +3914,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="26">
         <v>12</v>
       </c>
@@ -3971,7 +3961,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -4018,7 +4008,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="26">
         <v>14</v>
       </c>
@@ -4065,7 +4055,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A16" s="26">
         <v>15</v>
       </c>
@@ -4112,7 +4102,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A17" s="26">
         <v>16</v>
       </c>
@@ -4159,7 +4149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A18" s="26">
         <v>17</v>
       </c>
@@ -4206,7 +4196,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A19" s="26">
         <v>18</v>
       </c>
@@ -4253,7 +4243,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="33" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A20" s="26">
         <v>19</v>
       </c>
@@ -4300,7 +4290,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="26">
         <v>20</v>
       </c>
@@ -4347,7 +4337,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="26">
         <v>21</v>
       </c>
@@ -4394,7 +4384,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="26">
         <v>22</v>
       </c>
@@ -4441,7 +4431,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:15" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="26">
         <v>23</v>
       </c>
@@ -4488,7 +4478,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A25" s="26">
         <v>24</v>
       </c>
@@ -4535,7 +4525,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:15" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="26">
         <v>25</v>
       </c>
@@ -4582,7 +4572,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A27" s="26">
         <v>26</v>
       </c>
@@ -4629,7 +4619,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A28" s="26">
         <v>27</v>
       </c>
@@ -4676,7 +4666,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A29" s="26">
         <v>28</v>
       </c>
@@ -4723,7 +4713,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A30" s="26">
         <v>29</v>
       </c>
@@ -4770,7 +4760,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:15" ht="36" x14ac:dyDescent="0.15">
       <c r="A31" s="26">
         <v>30</v>
       </c>
@@ -4817,7 +4807,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="22" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A32" s="26">
         <v>31</v>
       </c>
@@ -5543,9 +5533,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5681,19 +5674,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0595DEA5-3BB4-4C08-A390-EF8B97AB3FDF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0517E4E2-4780-401D-9012-64C99AF61BEC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5717,9 +5706,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0517E4E2-4780-401D-9012-64C99AF61BEC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0595DEA5-3BB4-4C08-A390-EF8B97AB3FDF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>